<commit_message>
Release Aspose.Cells Cloud SDK 25.4.0
</commit_message>
<xml_diff>
--- a/TestData/BookText.xlsx
+++ b/TestData/BookText.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28502"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cells.cloud.family\cells.cloud\src\testdata\Cells\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3ED233-B373-452E-8103-C218AC290B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157085B9-9117-416A-AFD2-3A643EAEA5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="202401" sheetId="3" r:id="rId1"/>
     <sheet name="202407" sheetId="9" r:id="rId2"/>
     <sheet name="Text" sheetId="10" r:id="rId3"/>
+    <sheet name="split" sheetId="11" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Name_2">#REF!</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>Rank</t>
   </si>
@@ -100,6 +101,235 @@
   <si>
     <t xml:space="preserve">   Hi,     RoY   Wang.  hellow  word!         
 </t>
+  </si>
+  <si>
+    <t>To remove characters by position, select the range in Excel that contains the values you want to delete.</t>
+  </si>
+  <si>
+    <r>
+      <t>Click </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>Expand selection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t> to get the entire table selected automatically.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pick </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>The first N characters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t> to delete any number of characters at the beginning of cell contents in the selected range.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Select </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>The last N characters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t> to remove any number of characters at the end of each cell contents in your range.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>If you select </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>All characters before text</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>, any values before the specified character or string in the range will be deleted.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Selecting </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>All characters after text</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t> will let you remove everything after the specified character or string in the selected cells.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>You can also </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>Remove all substrings between value 1 and value 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>. For this, enter both values into the corresponding boxes. If you select the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>Including delimiters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t> option, the substring will be removed together with the values you entered. If you do not check it, the values will remain in the cells.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>To perform case-sensitive search, select the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>Case-sensitive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t> checkbox.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Select the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>Back up this worksheet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t> option to keep the original data intact.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Click the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t>Remove</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF333333"/>
+        <rFont val="Open Sans"/>
+      </rPr>
+      <t> button to see the results.</t>
+    </r>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>AB|CD|EF|GH</t>
+  </si>
+  <si>
+    <t>BA|DC|FE|HG</t>
   </si>
 </sst>
 </file>
@@ -112,7 +342,7 @@
     <numFmt numFmtId="166" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +390,22 @@
       <sz val="11"/>
       <color rgb="FF333A42"/>
       <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Open Sans"/>
     </font>
   </fonts>
   <fills count="3">
@@ -209,7 +455,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -220,11 +466,17 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -556,16 +808,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="4" spans="2:9" ht="15.75" thickBot="1">
@@ -1014,16 +1266,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="5" spans="2:9" ht="15.75" thickBot="1">
@@ -1450,20 +1702,127 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2036091A-1B06-4FA8-8B01-7CDD0E466B74}">
-  <dimension ref="D4:F4"/>
+  <dimension ref="D4:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="6.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="9" max="9" width="125.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:9" ht="270">
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9">
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9">
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" ht="16.5">
+      <c r="I9" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" ht="16.5">
+      <c r="I10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" ht="16.5">
+      <c r="I11" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" ht="16.5">
+      <c r="I12" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" ht="16.5">
+      <c r="I13" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" ht="16.5">
+      <c r="I14" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" ht="49.5">
+      <c r="I15" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="4:9" ht="16.5">
+      <c r="I16" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" ht="16.5">
+      <c r="I17" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" ht="16.5">
+      <c r="I19" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50EB8D3-1497-4E89-9A91-B9801C7B7858}">
+  <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:F4"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="4:6" ht="225">
-      <c r="D4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>19</v>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>